<commit_message>
add date of designation, include new districts
</commit_message>
<xml_diff>
--- a/lotarea 2016-10/data/Before and After Lotarea by Land Use Code 19v2.xlsx
+++ b/lotarea 2016-10/data/Before and After Lotarea by Land Use Code 19v2.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Mac\Home\Documents\DCP\db-pluto-research\lotarea 2016-10\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{AD3AD8E7-D995-4711-AAEC-C931A7B944FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C720531A-E707-4584-8F96-EB9A7601D3B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3323" yWindow="2062" windowWidth="16200" windowHeight="9398"/>
+    <workbookView xWindow="3323" yWindow="2062" windowWidth="16200" windowHeight="9398" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="landuse" sheetId="1" r:id="rId1"/>
+    <sheet name="Lotarea - Landuse" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>1 &amp; 2-Family</t>
   </si>
@@ -68,12 +68,15 @@
   </si>
   <si>
     <t>Land Use</t>
+  </si>
+  <si>
+    <t>Count of Records Changed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -554,7 +557,9 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -909,11 +914,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -922,9 +927,10 @@
     <col min="2" max="2" width="26.46484375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="25.265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" s="2" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>15</v>
       </c>
@@ -937,8 +943,11 @@
       <c r="D1" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -951,8 +960,11 @@
       <c r="D2" s="1">
         <v>5072</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E2" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -965,8 +977,11 @@
       <c r="D3" s="1">
         <v>3563176</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E3" s="1">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -979,8 +994,11 @@
       <c r="D4" s="1">
         <v>1583713</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E4" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -993,8 +1011,11 @@
       <c r="D5" s="1">
         <v>3239283</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E5" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1007,8 +1028,11 @@
       <c r="D6" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1021,8 +1045,11 @@
       <c r="D7" s="1">
         <v>-21726</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1035,8 +1062,11 @@
       <c r="D8" s="1">
         <v>151959603</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E8" s="1">
+        <v>1966</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1049,8 +1079,11 @@
       <c r="D9" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1063,8 +1096,11 @@
       <c r="D10" s="1">
         <v>272857</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E10" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1077,8 +1113,11 @@
       <c r="D11" s="1">
         <v>11758</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E11" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1091,8 +1130,11 @@
       <c r="D12" s="1">
         <v>4323367</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="E12" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1104,6 +1146,9 @@
       </c>
       <c r="D13" s="1">
         <v>1632893</v>
+      </c>
+      <c r="E13" s="1">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>